<commit_message>
Change price round to 10 decimal places
Some coins have very low prices so it's necessary to have high accuracy
</commit_message>
<xml_diff>
--- a/random_coins.xlsx
+++ b/random_coins.xlsx
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1904</v>
+        <v>512</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>43090</v>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1720</v>
+        <v>1839</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>43088</v>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1785</v>
+        <v>1659</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>43054</v>
@@ -501,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>576</v>
+        <v>693</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>43033</v>
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>495</v>
+        <v>870</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>43021</v>
@@ -529,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1454</v>
+        <v>1637</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>43005</v>
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1925</v>
+        <v>495</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>42999</v>
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1680</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>42987</v>
@@ -571,7 +571,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1697</v>
+        <v>463</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>42982</v>
@@ -585,7 +585,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1169</v>
+        <v>1027</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>42972</v>
@@ -599,7 +599,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1403</v>
+        <v>1274</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>42965</v>
@@ -613,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1518</v>
+        <v>372</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>43181</v>
@@ -627,7 +627,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1750</v>
+        <v>2544</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>43188</v>
@@ -641,7 +641,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2346</v>
+        <v>2087</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>43230</v>
@@ -655,7 +655,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>463</v>
+        <v>2638</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>43289</v>
@@ -669,7 +669,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1808</v>
+        <v>1586</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>43329</v>
@@ -683,7 +683,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1700</v>
+        <v>2469</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>43357</v>
@@ -697,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1789</v>
+        <v>2137</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>43444</v>
@@ -711,7 +711,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1975</v>
+        <v>1521</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>43452</v>
@@ -725,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2840</v>
+        <v>2682</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>43480</v>
@@ -739,7 +739,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>2502</v>
+        <v>2900</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>43515</v>
@@ -753,7 +753,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1765</v>
+        <v>1230</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>43545</v>
@@ -767,7 +767,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1903</v>
+        <v>1087</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>43584</v>
@@ -795,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1567</v>
+        <v>3437</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>43662</v>
@@ -809,7 +809,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1521</v>
+        <v>2405</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>43704</v>
@@ -823,7 +823,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>2308</v>
+        <v>1808</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>43739</v>
@@ -837,7 +837,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>3437</v>
+        <v>131</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>43767</v>
@@ -851,7 +851,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>3987</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>43756</v>
@@ -865,7 +865,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>2130</v>
+        <v>3873</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>43867</v>
@@ -879,7 +879,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1684</v>
+        <v>3704</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>43895</v>
@@ -893,7 +893,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>4846</v>
+        <v>2502</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>44063</v>
@@ -907,7 +907,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>512</v>
+        <v>5268</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>44138</v>
@@ -921,7 +921,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1896</v>
+        <v>1698</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>44202</v>
@@ -935,7 +935,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>6535</v>
+        <v>1975</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>44299</v>
@@ -949,7 +949,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>2469</v>
+        <v>5994</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>44408</v>
@@ -963,7 +963,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1414</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>43259</v>

</xml_diff>